<commit_message>
Add system type and enthalpy classifcation
</commit_message>
<xml_diff>
--- a/PowerDensityDatabase_MWilmarth-JStimac-GGanefianto-2020-WGC-Data.xlsx
+++ b/PowerDensityDatabase_MWilmarth-JStimac-GGanefianto-2020-WGC-Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irene/Dropbox (Personal)/PhD/Data-Analysis/PwrCap-PowerDensity-Public-GITREPO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4056AF6C-26A6-FE4F-8E2D-4ABFA7E4D5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCBBD1E-E82B-DA44-90AB-A9E985B2830C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27980" windowHeight="17540" xr2:uid="{6A508352-B733-C143-8C74-40F00ED77FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$113</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="127">
   <si>
     <t>Field</t>
   </si>
@@ -384,10 +385,40 @@
     <t>Arc</t>
   </si>
   <si>
-    <t>Not on plot</t>
-  </si>
-  <si>
     <t>Tectonic_setting_WGC2020</t>
+  </si>
+  <si>
+    <t>Deep circulation</t>
+  </si>
+  <si>
+    <t>System_type</t>
+  </si>
+  <si>
+    <t>Silicic intrusion</t>
+  </si>
+  <si>
+    <t>Deep circulation - magmatic</t>
+  </si>
+  <si>
+    <t>Rift - basaltic</t>
+  </si>
+  <si>
+    <t>Rift - silicic</t>
+  </si>
+  <si>
+    <t>Enthalpy</t>
+  </si>
+  <si>
+    <t>Vapor dominated</t>
+  </si>
+  <si>
+    <t>Hot water - low temperature</t>
+  </si>
+  <si>
+    <t>Hot water - intermediate temperature</t>
+  </si>
+  <si>
+    <t>Two-phase - liquid dominated</t>
   </si>
 </sst>
 </file>
@@ -755,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD43A95-036F-F94B-B598-5D110AD6DB9C}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,7 +801,7 @@
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,11 +812,16 @@
         <v>110</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -798,8 +834,14 @@
       <c r="D2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -809,11 +851,11 @@
       <c r="C3" s="1">
         <v>7.7824230129999998</v>
       </c>
-      <c r="D3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -823,11 +865,11 @@
       <c r="C4" s="1">
         <v>7.692307692</v>
       </c>
-      <c r="D4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -840,8 +882,14 @@
       <c r="D5" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -854,8 +902,14 @@
       <c r="D6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -868,8 +922,14 @@
       <c r="D7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -879,11 +939,14 @@
       <c r="C8" s="1">
         <v>19.047487929999999</v>
       </c>
-      <c r="D8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
@@ -893,11 +956,14 @@
       <c r="C9" s="1">
         <v>1.2176755690000001</v>
       </c>
-      <c r="D9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>74</v>
       </c>
@@ -910,8 +976,14 @@
       <c r="D10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -924,8 +996,14 @@
       <c r="D11" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>61</v>
       </c>
@@ -938,8 +1016,14 @@
       <c r="D12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -949,11 +1033,12 @@
       <c r="C13" s="1">
         <v>19.084308799999999</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="2"/>
+      <c r="F13" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
@@ -963,11 +1048,12 @@
       <c r="C14" s="1">
         <v>8.6666666669999994</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+      <c r="F14" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>96</v>
       </c>
@@ -980,8 +1066,14 @@
       <c r="D15" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -994,8 +1086,14 @@
       <c r="D16" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
@@ -1008,8 +1106,14 @@
       <c r="D17" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1022,8 +1126,14 @@
       <c r="D18" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
@@ -1036,8 +1146,14 @@
       <c r="D19" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1050,8 +1166,14 @@
       <c r="D20" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -1064,8 +1186,14 @@
       <c r="D21" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1078,8 +1206,14 @@
       <c r="D22" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>62</v>
       </c>
@@ -1092,8 +1226,14 @@
       <c r="D23" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
@@ -1106,8 +1246,14 @@
       <c r="D24" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
@@ -1120,8 +1266,14 @@
       <c r="D25" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
@@ -1134,8 +1286,14 @@
       <c r="D26" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
@@ -1148,8 +1306,14 @@
       <c r="D27" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -1162,8 +1326,14 @@
       <c r="D28" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -1176,8 +1346,14 @@
       <c r="D29" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
@@ -1190,8 +1366,14 @@
       <c r="D30" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>106</v>
       </c>
@@ -1204,8 +1386,14 @@
       <c r="D31" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>89</v>
       </c>
@@ -1218,8 +1406,14 @@
       <c r="D32" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>93</v>
       </c>
@@ -1229,11 +1423,15 @@
       <c r="C33" s="1">
         <v>1.483006201</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="2"/>
+      <c r="E33" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -1246,8 +1444,14 @@
       <c r="D34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1260,8 +1464,14 @@
       <c r="D35" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -1274,8 +1484,14 @@
       <c r="D36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>98</v>
       </c>
@@ -1288,8 +1504,14 @@
       <c r="D37" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>121</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>80</v>
       </c>
@@ -1302,8 +1524,11 @@
       <c r="D38" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>68</v>
       </c>
@@ -1316,8 +1541,11 @@
       <c r="D39" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
@@ -1330,8 +1558,14 @@
       <c r="D40" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -1344,8 +1578,14 @@
       <c r="D41" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>81</v>
       </c>
@@ -1358,8 +1598,14 @@
       <c r="D42" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
@@ -1372,8 +1618,14 @@
       <c r="D43" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
@@ -1386,8 +1638,14 @@
       <c r="D44" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
@@ -1400,8 +1658,14 @@
       <c r="D45" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -1414,8 +1678,14 @@
       <c r="D46" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>40</v>
       </c>
@@ -1428,8 +1698,14 @@
       <c r="D47" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>114</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -1442,8 +1718,14 @@
       <c r="D48" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>114</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -1456,8 +1738,14 @@
       <c r="D49" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
@@ -1470,8 +1758,14 @@
       <c r="D50" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>119</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
@@ -1484,8 +1778,14 @@
       <c r="D51" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>30</v>
       </c>
@@ -1498,8 +1798,14 @@
       <c r="D52" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
@@ -1512,8 +1818,14 @@
       <c r="D53" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>101</v>
       </c>
@@ -1526,8 +1838,14 @@
       <c r="D54" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>121</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -1540,8 +1858,14 @@
       <c r="D55" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>114</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>32</v>
       </c>
@@ -1554,8 +1878,14 @@
       <c r="D56" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>114</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
@@ -1568,8 +1898,14 @@
       <c r="D57" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -1582,8 +1918,14 @@
       <c r="D58" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>114</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -1596,8 +1938,14 @@
       <c r="D59" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>116</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>91</v>
       </c>
@@ -1610,8 +1958,14 @@
       <c r="D60" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>99</v>
       </c>
@@ -1624,8 +1978,14 @@
       <c r="D61" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>121</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>83</v>
       </c>
@@ -1638,8 +1998,11 @@
       <c r="D62" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F62" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>37</v>
       </c>
@@ -1652,8 +2015,14 @@
       <c r="D63" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>23</v>
       </c>
@@ -1666,8 +2035,14 @@
       <c r="D64" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>114</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>97</v>
       </c>
@@ -1680,8 +2055,14 @@
       <c r="D65" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>121</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>95</v>
       </c>
@@ -1694,8 +2075,14 @@
       <c r="D66" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" t="s">
+        <v>121</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>26</v>
       </c>
@@ -1708,8 +2095,14 @@
       <c r="D67" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>114</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>27</v>
       </c>
@@ -1722,8 +2115,14 @@
       <c r="D68" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>114</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>33</v>
       </c>
@@ -1736,8 +2135,14 @@
       <c r="D69" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>114</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>64</v>
       </c>
@@ -1750,8 +2155,14 @@
       <c r="D70" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" t="s">
+        <v>116</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>51</v>
       </c>
@@ -1764,8 +2175,14 @@
       <c r="D71" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" t="s">
+        <v>114</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>67</v>
       </c>
@@ -1778,8 +2195,14 @@
       <c r="D72" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" t="s">
+        <v>116</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>54</v>
       </c>
@@ -1792,8 +2215,14 @@
       <c r="D73" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>114</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>22</v>
       </c>
@@ -1806,8 +2235,14 @@
       <c r="D74" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>114</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>103</v>
       </c>
@@ -1820,8 +2255,11 @@
       <c r="D75" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F75" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>104</v>
       </c>
@@ -1831,11 +2269,11 @@
       <c r="C76" s="1">
         <v>4.423076923</v>
       </c>
-      <c r="D76" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F76" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>8</v>
       </c>
@@ -1848,8 +2286,14 @@
       <c r="D77" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>114</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>107</v>
       </c>
@@ -1862,8 +2306,14 @@
       <c r="D78" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" t="s">
+        <v>120</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>72</v>
       </c>
@@ -1876,8 +2326,14 @@
       <c r="D79" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>116</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>90</v>
       </c>
@@ -1890,8 +2346,14 @@
       <c r="D80" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>120</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>76</v>
       </c>
@@ -1904,8 +2366,14 @@
       <c r="D81" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" t="s">
+        <v>116</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>102</v>
       </c>
@@ -1918,8 +2386,14 @@
       <c r="D82" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>121</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>16</v>
       </c>
@@ -1932,8 +2406,14 @@
       <c r="D83" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" t="s">
+        <v>114</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>66</v>
       </c>
@@ -1946,8 +2426,11 @@
       <c r="D84" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F84" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>108</v>
       </c>
@@ -1960,8 +2443,11 @@
       <c r="D85" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F85" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>59</v>
       </c>
@@ -1974,8 +2460,14 @@
       <c r="D86" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
+        <v>116</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>44</v>
       </c>
@@ -1988,8 +2480,14 @@
       <c r="D87" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>114</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>10</v>
       </c>
@@ -2002,8 +2500,14 @@
       <c r="D88" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" t="s">
+        <v>114</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>21</v>
       </c>
@@ -2016,8 +2520,14 @@
       <c r="D89" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" t="s">
+        <v>114</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>84</v>
       </c>
@@ -2030,8 +2540,14 @@
       <c r="D90" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90" t="s">
+        <v>119</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>24</v>
       </c>
@@ -2044,8 +2560,14 @@
       <c r="D91" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91" t="s">
+        <v>114</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>35</v>
       </c>
@@ -2058,8 +2580,14 @@
       <c r="D92" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92" t="s">
+        <v>114</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>92</v>
       </c>
@@ -2072,8 +2600,14 @@
       <c r="D93" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93" t="s">
+        <v>120</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>36</v>
       </c>
@@ -2086,8 +2620,14 @@
       <c r="D94" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94" t="s">
+        <v>114</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>49</v>
       </c>
@@ -2100,8 +2640,14 @@
       <c r="D95" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95" t="s">
+        <v>114</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>53</v>
       </c>
@@ -2114,8 +2660,14 @@
       <c r="D96" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96" t="s">
+        <v>114</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>82</v>
       </c>
@@ -2128,8 +2680,11 @@
       <c r="D97" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F97" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>63</v>
       </c>
@@ -2142,8 +2697,14 @@
       <c r="D98" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98" t="s">
+        <v>116</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>28</v>
       </c>
@@ -2156,8 +2717,14 @@
       <c r="D99" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99" t="s">
+        <v>114</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>19</v>
       </c>
@@ -2170,8 +2737,11 @@
       <c r="D100" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F100" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>12</v>
       </c>
@@ -2184,8 +2754,14 @@
       <c r="D101" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101" t="s">
+        <v>114</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>71</v>
       </c>
@@ -2195,11 +2771,11 @@
       <c r="C102" s="1">
         <v>4.3213774230000004</v>
       </c>
-      <c r="D102" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F102" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>100</v>
       </c>
@@ -2212,8 +2788,14 @@
       <c r="D103" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103" t="s">
+        <v>121</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>15</v>
       </c>
@@ -2226,8 +2808,14 @@
       <c r="D104" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104" t="s">
+        <v>114</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>57</v>
       </c>
@@ -2240,8 +2828,14 @@
       <c r="D105" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105" t="s">
+        <v>116</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>29</v>
       </c>
@@ -2254,8 +2848,14 @@
       <c r="D106" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106" t="s">
+        <v>114</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>31</v>
       </c>
@@ -2268,8 +2868,14 @@
       <c r="D107" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107" t="s">
+        <v>114</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>79</v>
       </c>
@@ -2282,8 +2888,11 @@
       <c r="D108" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F108" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>7</v>
       </c>
@@ -2296,18 +2905,24 @@
       <c r="D109" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109" t="s">
+        <v>114</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2317,10 +2932,28 @@
       <c r="B113" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D113" xr:uid="{52D25DE7-05A2-4A44-81A2-E14FDA749211}"/>
+  <autoFilter ref="A1:F113" xr:uid="{DAD43A95-036F-F94B-B598-5D110AD6DB9C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F113">
+      <sortCondition ref="A1:A113"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D113">
     <sortCondition ref="A2:A113"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34521E74-5013-9D46-9995-6C29A3A7E3A4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>